<commit_message>
Added Nacubo GL Account Category
</commit_message>
<xml_diff>
--- a/src/main/java/TestSuite/MDOT/TestCases/MDOT/Login_Login.xlsx
+++ b/src/main/java/TestSuite/MDOT/TestCases/MDOT/Login_Login.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24729"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC9927D-C129-4FB6-A3A5-DBD71A93ACF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BC51B93-6655-4726-8486-44F24449DB48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestSteps" sheetId="4" r:id="rId1"/>
@@ -166,7 +166,7 @@
     <t>athakur</t>
   </si>
   <si>
-    <t>Worsts80#Picard</t>
+    <t>Adarsh80#Picard</t>
   </si>
 </sst>
 </file>
@@ -631,8 +631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:C7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -776,8 +776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1128,21 +1128,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009AB4AFD5B95DA74C9A5B41FD6646044C" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="93f9b83cafbf659b556859d3b1438975">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="89d62139-6d9b-4693-b5fe-6b91abfb079e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="14da90777f3d3c2815d7913a0d1ee4cf" ns2:_="">
     <xsd:import namespace="89d62139-6d9b-4693-b5fe-6b91abfb079e"/>
@@ -1274,24 +1259,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B671AFB-4015-4766-9DDE-AAF09D7A20BB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A379EDB-DDBF-4E96-9D13-E82BA1A4C408}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AE96A698-88B9-42A4-9502-16538EAC77A8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1307,4 +1290,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A379EDB-DDBF-4E96-9D13-E82BA1A4C408}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B671AFB-4015-4766-9DDE-AAF09D7A20BB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>